<commit_message>
update template, fix return picking
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_stock/static/src/xlsx/template_ycnk.xlsx
+++ b/addons/custom/forlife_stock/static/src/xlsx/template_ycnk.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Project\m_onnet_odoo_mfl2201er\addons\custom\forlife_stock\static\src\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FORLIFE\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9BA8DA8-7EFE-498E-B265-8A5FC938A029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{34DD19CF-FB00-4A69-95EA-F68878B1CFA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3432D23C-C5BB-448A-8A00-3FD4AFE0BF35}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="19">
   <si>
     <t>Nhập khác</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>T2</t>
-  </si>
-  <si>
-    <t>Đơn vị</t>
   </si>
   <si>
     <t>1521_NPL</t>
@@ -127,7 +124,22 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Chi tiết / Đơn vị </t>
+      <t>Chi tiết / Loại lý do</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (*)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chi tiết / Lý do nhập </t>
     </r>
     <r>
       <rPr>
@@ -142,7 +154,7 @@
   </si>
   <si>
     <r>
-      <t>Chi tiết / Loại lý do</t>
+      <t>Chi tiết / Đến kho</t>
     </r>
     <r>
       <rPr>
@@ -156,36 +168,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Chi tiết / Lý do nhập </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>(*)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Chi tiết / Đến kho</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> (*)</t>
-    </r>
-  </si>
-  <si>
     <t>Chi tiết / Mã vụ việc</t>
   </si>
   <si>
@@ -193,6 +175,9 @@
   </si>
   <si>
     <t>Chi tiết / Trung tâm chi phí</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -658,68 +643,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E024EC5C-06AB-479A-BE4E-6B23C2BEC4B7}">
-  <dimension ref="A1:L5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="46.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="E1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="12">
         <v>44655</v>
       </c>
@@ -727,63 +708,65 @@
         <v>0</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="13"/>
+        <v>4</v>
+      </c>
+      <c r="D2" s="13">
+        <v>45163</v>
+      </c>
       <c r="E2" s="5">
         <v>10</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="8">
+      <c r="H2" s="8">
         <v>1075</v>
       </c>
-      <c r="J2" s="7">
+      <c r="I2" s="7">
         <v>1405000161</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="7">
+      <c r="K2" s="7">
         <v>1511020000</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="6"/>
       <c r="C3" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="13"/>
+        <v>5</v>
+      </c>
+      <c r="D3" s="13">
+        <v>45164</v>
+      </c>
       <c r="E3" s="5">
         <v>15</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="8">
+      <c r="H3" s="8">
         <v>1076</v>
       </c>
-      <c r="J3" s="7">
+      <c r="I3" s="7">
         <v>1405000161</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L3" s="7">
+      <c r="K3" s="7">
         <v>1511020000</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="12">
         <v>44655</v>
       </c>
@@ -791,66 +774,68 @@
         <v>0</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="D4" s="13">
+        <v>45165</v>
+      </c>
       <c r="E4" s="5">
         <v>20</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="8">
+      <c r="H4" s="8">
         <v>1077</v>
       </c>
-      <c r="J4" s="7">
+      <c r="I4" s="7">
         <v>1405000161</v>
       </c>
-      <c r="K4" s="7" t="s">
+      <c r="J4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="L4" s="7">
+      <c r="K4" s="7">
         <v>1511020000</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="6"/>
       <c r="C5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="13"/>
+        <v>4</v>
+      </c>
+      <c r="D5" s="13">
+        <v>45166</v>
+      </c>
       <c r="E5" s="5">
         <v>25</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I5" s="8">
+      <c r="H5" s="8">
         <v>1078</v>
       </c>
-      <c r="J5" s="7">
+      <c r="I5" s="7">
         <v>1405000161</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="J5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="L5" s="7">
+      <c r="K5" s="7">
         <v>1511020000</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{45161D29-6ECE-4EB9-AD82-96C5E3251BD5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Nhập khác, Xuất khác"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fix import other request
</commit_message>
<xml_diff>
--- a/addons/custom/forlife_stock/static/src/xlsx/template_ycnk.xlsx
+++ b/addons/custom/forlife_stock/static/src/xlsx/template_ycnk.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FORLIFE\TAI LIEU DU AN\ERP\Template import_Odoo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aht\Desktop\Forlife\m_onnet_odoo_mfl2201er\addons\custom\forlife_stock\static\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -206,7 +206,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -230,7 +230,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -254,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -278,7 +278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -302,7 +302,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -326,7 +326,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -350,7 +350,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="S1" authorId="0" shapeId="0">
+    <comment ref="R1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -379,7 +379,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="618">
   <si>
     <t>Nhập khác</t>
   </si>
@@ -2329,9 +2329,6 @@
   </si>
   <si>
     <t>Địa điểm xuât NPL</t>
-  </si>
-  <si>
-    <t>Ghi chú</t>
   </si>
 </sst>
 </file>
@@ -2949,28 +2946,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>7</v>
       </c>
@@ -2998,38 +2995,35 @@
       <c r="I1" s="42" t="s">
         <v>616</v>
       </c>
-      <c r="J1" s="42" t="s">
-        <v>618</v>
-      </c>
-      <c r="K1" s="43" t="s">
+      <c r="J1" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="K1" s="39" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="44">
         <v>44655</v>
       </c>
@@ -3043,36 +3037,35 @@
       <c r="G2" s="45"/>
       <c r="H2" s="45"/>
       <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="6" t="s">
+      <c r="J2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="40">
+      <c r="K2" s="40">
         <v>45163</v>
       </c>
-      <c r="M2" s="2">
+      <c r="L2" s="2">
         <v>10</v>
       </c>
+      <c r="M2" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="N2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="4">
+      <c r="O2" s="4">
         <v>1075</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="P2" s="3">
         <v>1405000161</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="3">
+      <c r="R2" s="3">
         <v>1511020000</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="46"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47"/>
@@ -3082,36 +3075,35 @@
       <c r="G3" s="47"/>
       <c r="H3" s="47"/>
       <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L3" s="40">
+      <c r="K3" s="40">
         <v>45164</v>
       </c>
-      <c r="M3" s="2">
+      <c r="L3" s="2">
         <v>15</v>
       </c>
+      <c r="M3" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="N3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P3" s="4">
+      <c r="O3" s="4">
         <v>1076</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="P3" s="3">
         <v>1405000161</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="Q3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S3" s="3">
+      <c r="R3" s="3">
         <v>1511020000</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="44">
         <v>44655</v>
       </c>
@@ -3125,36 +3117,35 @@
       <c r="G4" s="45"/>
       <c r="H4" s="45"/>
       <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
-      <c r="K4" s="6" t="s">
+      <c r="J4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="40">
+      <c r="K4" s="40">
         <v>45165</v>
       </c>
-      <c r="M4" s="2">
+      <c r="L4" s="2">
         <v>20</v>
       </c>
+      <c r="M4" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="N4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="4">
+      <c r="O4" s="4">
         <v>1077</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="P4" s="3">
         <v>1405000161</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="S4" s="3">
+      <c r="R4" s="3">
         <v>1511020000</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="46"/>
       <c r="B5" s="47"/>
       <c r="C5" s="47"/>
@@ -3164,39 +3155,38 @@
       <c r="G5" s="47"/>
       <c r="H5" s="47"/>
       <c r="I5" s="47"/>
-      <c r="J5" s="47"/>
-      <c r="K5" s="6" t="s">
+      <c r="J5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="40">
+      <c r="K5" s="40">
         <v>45166</v>
       </c>
-      <c r="M5" s="2">
+      <c r="L5" s="2">
         <v>25</v>
       </c>
+      <c r="M5" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="N5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="P5" s="4">
+      <c r="O5" s="4">
         <v>1078</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="P5" s="3">
         <v>1405000161</v>
       </c>
-      <c r="R5" s="3" t="s">
+      <c r="Q5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="S5" s="3">
+      <c r="R5" s="3">
         <v>1511020000</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:J2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:I2">
       <formula1>"Nhập khác, Xuất khác"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>